<commit_message>
Add data for 2023-06-28
</commit_message>
<xml_diff>
--- a/output/cta-violent-crime-full-year.xlsx
+++ b/output/cta-violent-crime-full-year.xlsx
@@ -25,36 +25,36 @@
     <sheet name="United Center" sheetId="16" r:id="rId16"/>
     <sheet name="Ashburn" sheetId="17" r:id="rId17"/>
     <sheet name="South Shore" sheetId="18" r:id="rId18"/>
-    <sheet name="West Pullman" sheetId="19" r:id="rId19"/>
-    <sheet name="Belmont Cragin" sheetId="20" r:id="rId20"/>
-    <sheet name="Wrigleyville" sheetId="21" r:id="rId21"/>
-    <sheet name="Bucktown" sheetId="22" r:id="rId22"/>
-    <sheet name="West Loop" sheetId="23" r:id="rId23"/>
-    <sheet name="Fuller Park" sheetId="24" r:id="rId24"/>
-    <sheet name="Roseland" sheetId="25" r:id="rId25"/>
-    <sheet name="Austin" sheetId="26" r:id="rId26"/>
-    <sheet name="Little Village" sheetId="27" r:id="rId27"/>
-    <sheet name="Little Italy, UIC" sheetId="28" r:id="rId28"/>
-    <sheet name="Archer Heights" sheetId="29" r:id="rId29"/>
-    <sheet name="Gage Park" sheetId="30" r:id="rId30"/>
-    <sheet name="Albany Park" sheetId="31" r:id="rId31"/>
-    <sheet name="Auburn Gresham" sheetId="32" r:id="rId32"/>
-    <sheet name="North Lawndale" sheetId="33" r:id="rId33"/>
-    <sheet name="Chicago Lawn" sheetId="34" r:id="rId34"/>
-    <sheet name="Hyde Park" sheetId="35" r:id="rId35"/>
-    <sheet name="Woodlawn" sheetId="36" r:id="rId36"/>
-    <sheet name="Uptown" sheetId="37" r:id="rId37"/>
-    <sheet name="East Side" sheetId="38" r:id="rId38"/>
-    <sheet name="South Deering" sheetId="39" r:id="rId39"/>
-    <sheet name="West Elsdon" sheetId="40" r:id="rId40"/>
-    <sheet name="Near South Side" sheetId="41" r:id="rId41"/>
-    <sheet name="Hermosa" sheetId="42" r:id="rId42"/>
-    <sheet name="Lincoln Park" sheetId="43" r:id="rId43"/>
-    <sheet name="Avalon Park" sheetId="44" r:id="rId44"/>
-    <sheet name="Streeterville" sheetId="45" r:id="rId45"/>
-    <sheet name="New City" sheetId="46" r:id="rId46"/>
-    <sheet name="Portage Park" sheetId="47" r:id="rId47"/>
-    <sheet name="Sheffield &amp; DePaul" sheetId="48" r:id="rId48"/>
+    <sheet name="Sheffield &amp; DePaul" sheetId="19" r:id="rId19"/>
+    <sheet name="West Pullman" sheetId="20" r:id="rId20"/>
+    <sheet name="Belmont Cragin" sheetId="21" r:id="rId21"/>
+    <sheet name="Wrigleyville" sheetId="22" r:id="rId22"/>
+    <sheet name="Bucktown" sheetId="23" r:id="rId23"/>
+    <sheet name="West Loop" sheetId="24" r:id="rId24"/>
+    <sheet name="Fuller Park" sheetId="25" r:id="rId25"/>
+    <sheet name="Roseland" sheetId="26" r:id="rId26"/>
+    <sheet name="Austin" sheetId="27" r:id="rId27"/>
+    <sheet name="Little Village" sheetId="28" r:id="rId28"/>
+    <sheet name="Little Italy, UIC" sheetId="29" r:id="rId29"/>
+    <sheet name="Archer Heights" sheetId="30" r:id="rId30"/>
+    <sheet name="Gage Park" sheetId="31" r:id="rId31"/>
+    <sheet name="Albany Park" sheetId="32" r:id="rId32"/>
+    <sheet name="Auburn Gresham" sheetId="33" r:id="rId33"/>
+    <sheet name="North Lawndale" sheetId="34" r:id="rId34"/>
+    <sheet name="Chicago Lawn" sheetId="35" r:id="rId35"/>
+    <sheet name="Hyde Park" sheetId="36" r:id="rId36"/>
+    <sheet name="Woodlawn" sheetId="37" r:id="rId37"/>
+    <sheet name="Uptown" sheetId="38" r:id="rId38"/>
+    <sheet name="East Side" sheetId="39" r:id="rId39"/>
+    <sheet name="South Deering" sheetId="40" r:id="rId40"/>
+    <sheet name="West Elsdon" sheetId="41" r:id="rId41"/>
+    <sheet name="Near South Side" sheetId="42" r:id="rId42"/>
+    <sheet name="Hermosa" sheetId="43" r:id="rId43"/>
+    <sheet name="Lincoln Park" sheetId="44" r:id="rId44"/>
+    <sheet name="Avalon Park" sheetId="45" r:id="rId45"/>
+    <sheet name="Streeterville" sheetId="46" r:id="rId46"/>
+    <sheet name="New City" sheetId="47" r:id="rId47"/>
+    <sheet name="Portage Park" sheetId="48" r:id="rId48"/>
     <sheet name="Douglas" sheetId="49" r:id="rId49"/>
     <sheet name="Brighton Park" sheetId="50" r:id="rId50"/>
     <sheet name="Lincoln Square" sheetId="51" r:id="rId51"/>
@@ -996,7 +996,7 @@
         <v>521</v>
       </c>
       <c r="J6">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1028,7 +1028,7 @@
         <v>873</v>
       </c>
       <c r="J7">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -2706,13 +2706,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2760,10 +2760,22 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="H2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
     </row>
@@ -2774,78 +2786,95 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4672,7 +4701,7 @@
         <v>19</v>
       </c>
       <c r="J70">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -5463,7 +5492,7 @@
         <v>873</v>
       </c>
       <c r="J98">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -5572,6 +5601,155 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5692,7 +5870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -5864,7 +6042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -5968,7 +6146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -6151,7 +6329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6326,7 +6504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -6536,7 +6714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6738,7 +6916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -6883,7 +7061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -7060,90 +7238,6 @@
       </c>
       <c r="J6">
         <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7325,6 +7419,90 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7497,7 +7675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -7646,190 +7824,6 @@
       </c>
       <c r="I6">
         <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>8</v>
-      </c>
-      <c r="G5">
-        <v>7</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -7894,28 +7888,25 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -7926,32 +7917,32 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3">
         <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
@@ -7960,31 +7951,31 @@
         <v>5</v>
       </c>
       <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>28</v>
-      </c>
-      <c r="E5">
-        <v>21</v>
-      </c>
       <c r="F5">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7992,31 +7983,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C6">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F6">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8080,17 +8071,29 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
       <c r="G2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -8098,25 +8101,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -8129,7 +8129,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
@@ -8138,28 +8138,28 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -8173,25 +8173,25 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="G6">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -8203,132 +8203,6 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -8384,20 +8258,17 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
+      <c r="D2">
         <v>1</v>
       </c>
       <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -8411,19 +8282,22 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -8433,10 +8307,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -8448,25 +8319,25 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -8477,30 +8348,156 @@
         <v>6</v>
       </c>
       <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>16</v>
       </c>
-      <c r="C6">
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
       <c r="H6">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I6">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
     </row>
@@ -8566,13 +8563,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -8582,9 +8573,6 @@
       </c>
       <c r="G2">
         <v>2</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -8594,36 +8582,39 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
@@ -8632,31 +8623,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>9</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
       <c r="F5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -8664,31 +8655,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>11</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8697,6 +8688,193 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -8782,146 +8960,6 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
         <v>1</v>
       </c>
     </row>
@@ -9113,6 +9151,146 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9227,7 +9405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -9399,7 +9577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -9485,7 +9663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -9648,7 +9826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -9764,7 +9942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -9873,7 +10051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -10021,7 +10199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -10132,184 +10310,6 @@
       </c>
       <c r="G6">
         <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -12967,6 +12967,9 @@
       <c r="I4">
         <v>17</v>
       </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
@@ -12997,7 +13000,7 @@
         <v>19</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-06-29
</commit_message>
<xml_diff>
--- a/output/cta-violent-crime-full-year.xlsx
+++ b/output/cta-violent-crime-full-year.xlsx
@@ -20,8 +20,8 @@
     <sheet name="South Chicago" sheetId="11" r:id="rId11"/>
     <sheet name="Garfield Park" sheetId="12" r:id="rId12"/>
     <sheet name="Armour Square" sheetId="13" r:id="rId13"/>
-    <sheet name="Rush &amp; Division" sheetId="14" r:id="rId14"/>
-    <sheet name="Uptown" sheetId="15" r:id="rId15"/>
+    <sheet name="Uptown" sheetId="14" r:id="rId14"/>
+    <sheet name="Rush &amp; Division" sheetId="15" r:id="rId15"/>
     <sheet name="Loop" sheetId="16" r:id="rId16"/>
     <sheet name="Chatham" sheetId="17" r:id="rId17"/>
     <sheet name="United Center" sheetId="18" r:id="rId18"/>
@@ -1781,6 +1781,196 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1942,196 +2132,6 @@
       </c>
       <c r="J5">
         <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>22</v>
-      </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-08
</commit_message>
<xml_diff>
--- a/output/cta-violent-crime-full-year.xlsx
+++ b/output/cta-violent-crime-full-year.xlsx
@@ -19,39 +19,39 @@
     <sheet name="Humboldt Park" sheetId="10" r:id="rId10"/>
     <sheet name="South Chicago" sheetId="11" r:id="rId11"/>
     <sheet name="Garfield Park" sheetId="12" r:id="rId12"/>
-    <sheet name="Armour Square" sheetId="13" r:id="rId13"/>
-    <sheet name="Rush &amp; Division" sheetId="14" r:id="rId14"/>
-    <sheet name="Loop" sheetId="15" r:id="rId15"/>
-    <sheet name="Chatham" sheetId="16" r:id="rId16"/>
-    <sheet name="Uptown" sheetId="17" r:id="rId17"/>
-    <sheet name="United Center" sheetId="18" r:id="rId18"/>
-    <sheet name="Ashburn" sheetId="19" r:id="rId19"/>
-    <sheet name="South Shore" sheetId="20" r:id="rId20"/>
+    <sheet name="Rush &amp; Division" sheetId="13" r:id="rId13"/>
+    <sheet name="Loop" sheetId="14" r:id="rId14"/>
+    <sheet name="Chatham" sheetId="15" r:id="rId15"/>
+    <sheet name="United Center" sheetId="16" r:id="rId16"/>
+    <sheet name="Ashburn" sheetId="17" r:id="rId17"/>
+    <sheet name="South Shore" sheetId="18" r:id="rId18"/>
+    <sheet name="Austin" sheetId="19" r:id="rId19"/>
+    <sheet name="Lincoln Park" sheetId="20" r:id="rId20"/>
     <sheet name="River North" sheetId="21" r:id="rId21"/>
-    <sheet name="Austin" sheetId="22" r:id="rId22"/>
-    <sheet name="Lincoln Park" sheetId="23" r:id="rId23"/>
-    <sheet name="Printers Row" sheetId="24" r:id="rId24"/>
-    <sheet name="Lake View" sheetId="25" r:id="rId25"/>
-    <sheet name="Fuller Park" sheetId="26" r:id="rId26"/>
-    <sheet name="Old Town" sheetId="27" r:id="rId27"/>
-    <sheet name="Logan Square" sheetId="28" r:id="rId28"/>
-    <sheet name="Irving Park" sheetId="29" r:id="rId29"/>
-    <sheet name="South Deering" sheetId="30" r:id="rId30"/>
-    <sheet name="Chinatown" sheetId="31" r:id="rId31"/>
-    <sheet name="Rogers Park" sheetId="32" r:id="rId32"/>
-    <sheet name="Belmont Cragin" sheetId="33" r:id="rId33"/>
-    <sheet name="Norwood Park" sheetId="34" r:id="rId34"/>
-    <sheet name="Edgewater" sheetId="35" r:id="rId35"/>
-    <sheet name="Little Italy, UIC" sheetId="36" r:id="rId36"/>
-    <sheet name="Bucktown" sheetId="37" r:id="rId37"/>
-    <sheet name="West Pullman" sheetId="38" r:id="rId38"/>
-    <sheet name="Roseland" sheetId="39" r:id="rId39"/>
-    <sheet name="Sheffield &amp; DePaul" sheetId="40" r:id="rId40"/>
-    <sheet name="Albany Park" sheetId="41" r:id="rId41"/>
-    <sheet name="Riverdale" sheetId="42" r:id="rId42"/>
-    <sheet name="Auburn Gresham" sheetId="43" r:id="rId43"/>
-    <sheet name="Douglas" sheetId="44" r:id="rId44"/>
-    <sheet name="Chicago Lawn" sheetId="45" r:id="rId45"/>
+    <sheet name="Printers Row" sheetId="22" r:id="rId22"/>
+    <sheet name="Lake View" sheetId="23" r:id="rId23"/>
+    <sheet name="Fuller Park" sheetId="24" r:id="rId24"/>
+    <sheet name="Old Town" sheetId="25" r:id="rId25"/>
+    <sheet name="Logan Square" sheetId="26" r:id="rId26"/>
+    <sheet name="Uptown" sheetId="27" r:id="rId27"/>
+    <sheet name="Irving Park" sheetId="28" r:id="rId28"/>
+    <sheet name="South Deering" sheetId="29" r:id="rId29"/>
+    <sheet name="Chinatown" sheetId="30" r:id="rId30"/>
+    <sheet name="Rogers Park" sheetId="31" r:id="rId31"/>
+    <sheet name="Belmont Cragin" sheetId="32" r:id="rId32"/>
+    <sheet name="Norwood Park" sheetId="33" r:id="rId33"/>
+    <sheet name="Edgewater" sheetId="34" r:id="rId34"/>
+    <sheet name="Little Italy, UIC" sheetId="35" r:id="rId35"/>
+    <sheet name="Bucktown" sheetId="36" r:id="rId36"/>
+    <sheet name="West Pullman" sheetId="37" r:id="rId37"/>
+    <sheet name="Roseland" sheetId="38" r:id="rId38"/>
+    <sheet name="Sheffield &amp; DePaul" sheetId="39" r:id="rId39"/>
+    <sheet name="Albany Park" sheetId="40" r:id="rId40"/>
+    <sheet name="Riverdale" sheetId="41" r:id="rId41"/>
+    <sheet name="Auburn Gresham" sheetId="42" r:id="rId42"/>
+    <sheet name="Douglas" sheetId="43" r:id="rId43"/>
+    <sheet name="Chicago Lawn" sheetId="44" r:id="rId44"/>
+    <sheet name="Armour Square" sheetId="45" r:id="rId45"/>
     <sheet name="West Loop" sheetId="46" r:id="rId46"/>
     <sheet name="Lincoln Square" sheetId="47" r:id="rId47"/>
     <sheet name="Woodlawn" sheetId="48" r:id="rId48"/>
@@ -1603,184 +1603,6 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1942,6 +1764,231 @@
       </c>
       <c r="J5">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>22</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="J3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>44</v>
+      </c>
+      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="E6">
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <v>69</v>
+      </c>
+      <c r="G6">
+        <v>57</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>62</v>
+      </c>
+      <c r="D7">
+        <v>79</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>92</v>
+      </c>
+      <c r="G7">
+        <v>88</v>
+      </c>
+      <c r="H7">
+        <v>118</v>
+      </c>
+      <c r="I7">
+        <v>130</v>
+      </c>
+      <c r="J7">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2005,32 +2052,29 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2038,57 +2082,39 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="H3">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
+      <c r="B4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2101,7 +2127,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
@@ -2110,31 +2136,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="G6">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2142,31 +2168,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E7">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="F7">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="G7">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="H7">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="I7">
-        <v>130</v>
+        <v>24</v>
       </c>
       <c r="J7">
-        <v>68</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2176,13 +2202,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2234,143 +2260,109 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>29</v>
-      </c>
-      <c r="E7">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>26</v>
-      </c>
-      <c r="G7">
-        <v>25</v>
-      </c>
-      <c r="H7">
-        <v>13</v>
-      </c>
-      <c r="I7">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2380,13 +2372,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2434,133 +2426,95 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>22</v>
-      </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2624,6 +2578,9 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -2631,42 +2588,51 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
       <c r="C3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2674,31 +2640,31 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2706,31 +2672,31 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J5">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2740,13 +2706,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2794,95 +2760,145 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
       <c r="C2">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
       <c r="D3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>2</v>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>57</v>
+      </c>
+      <c r="F6">
+        <v>53</v>
+      </c>
+      <c r="G6">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>63</v>
+      </c>
+      <c r="I6">
+        <v>44</v>
+      </c>
+      <c r="J6">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -5612,13 +5628,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -5666,28 +5682,16 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>2</v>
       </c>
     </row>
@@ -5695,96 +5699,89 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -5978,13 +5975,13 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -6032,32 +6029,14 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -6065,45 +6044,45 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>8</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -6111,66 +6090,34 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="J5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>32</v>
-      </c>
-      <c r="C6">
-        <v>40</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-      <c r="E6">
-        <v>57</v>
-      </c>
-      <c r="F6">
-        <v>53</v>
-      </c>
-      <c r="G6">
-        <v>34</v>
-      </c>
-      <c r="H6">
-        <v>63</v>
-      </c>
-      <c r="I6">
-        <v>44</v>
-      </c>
-      <c r="J6">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6234,41 +6181,74 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
       <c r="F3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
@@ -6276,32 +6256,29 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6312,28 +6289,28 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -6342,6 +6319,181 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -6397,13 +6549,19 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -6414,14 +6572,26 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
       <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6429,31 +6599,31 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6461,31 +6631,31 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I5">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6493,7 +6663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6550,25 +6720,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -6578,45 +6742,36 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -6624,29 +6779,32 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
       <c r="C5">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6657,28 +6815,28 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F6">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="I6">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -6686,7 +6844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6694,7 +6852,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -6742,13 +6900,31 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -6756,39 +6932,36 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -6797,28 +6970,28 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -6832,198 +7005,28 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>22</v>
+      </c>
+      <c r="H6">
         <v>14</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>10</v>
       </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>12</v>
-      </c>
       <c r="J6">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>18</v>
-      </c>
-      <c r="G4">
-        <v>12</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <v>17</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
         <v>9</v>
-      </c>
-      <c r="E5">
-        <v>19</v>
-      </c>
-      <c r="F5">
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>17</v>
-      </c>
-      <c r="I5">
-        <v>19</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -7091,25 +7094,31 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3">
         <v>1</v>
       </c>
@@ -7119,27 +7128,21 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
@@ -7148,31 +7151,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -7183,28 +7186,28 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J6">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -7214,7 +7217,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7228,11 +7231,9 @@
     <col min="6" max="6" width="4.7109375" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7246,96 +7247,72 @@
         <v>2017</v>
       </c>
       <c r="E1" s="1">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F1" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G1" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -7344,48 +7321,33 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7567,7 +7529,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7581,9 +7543,11 @@
     <col min="6" max="6" width="4.7109375" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7597,92 +7561,92 @@
         <v>2017</v>
       </c>
       <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
         <v>2019</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2020</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2021</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="E3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -7691,13 +7655,51 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>17</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -7761,51 +7763,69 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
       <c r="E2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -7821,31 +7841,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -7853,31 +7873,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>23</v>
+      </c>
+      <c r="J7">
         <v>8</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>12</v>
-      </c>
-      <c r="I7">
-        <v>17</v>
-      </c>
-      <c r="J7">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -7887,7 +7907,7 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7901,11 +7921,9 @@
     <col min="6" max="6" width="4.7109375" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7922,160 +7940,86 @@
         <v>2018</v>
       </c>
       <c r="F1" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G1" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
       <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
       <c r="E3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>13</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>15</v>
-      </c>
-      <c r="D7">
-        <v>17</v>
-      </c>
-      <c r="E7">
-        <v>21</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>21</v>
-      </c>
-      <c r="H7">
-        <v>18</v>
-      </c>
-      <c r="I7">
-        <v>23</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8106,22 +8050,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="C1" s="1">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="D1" s="1">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="E1" s="1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F1" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G1" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="H1" s="1">
         <v>2023</v>
@@ -8139,8 +8083,11 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -8150,7 +8097,10 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
     </row>
@@ -8159,16 +8109,16 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -8179,22 +8129,22 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -8206,134 +8156,6 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -8503,7 +8325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -8687,7 +8509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -8791,7 +8613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -8940,7 +8762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -9143,6 +8965,184 @@
       </c>
       <c r="J7">
         <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -9333,184 +9333,6 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9665,7 +9487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -9798,7 +9620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -9982,7 +9804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -10135,6 +9957,184 @@
         <v>7</v>
       </c>
       <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
         <v>2</v>
       </c>
     </row>
@@ -10199,17 +10199,23 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -10217,30 +10223,24 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
         <v>1</v>
       </c>
     </row>
@@ -10248,7 +10248,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
@@ -10257,31 +10257,31 @@
         <v>5</v>
       </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="J5">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10289,31 +10289,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
         <v>8</v>
       </c>
-      <c r="G6">
-        <v>13</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
       <c r="I6">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-11
</commit_message>
<xml_diff>
--- a/output/cta-violent-crime-full-year.xlsx
+++ b/output/cta-violent-crime-full-year.xlsx
@@ -19,23 +19,23 @@
     <sheet name="Humboldt Park" sheetId="10" r:id="rId10"/>
     <sheet name="South Chicago" sheetId="11" r:id="rId11"/>
     <sheet name="Garfield Park" sheetId="12" r:id="rId12"/>
-    <sheet name="Armour Square" sheetId="13" r:id="rId13"/>
-    <sheet name="Rush &amp; Division" sheetId="14" r:id="rId14"/>
-    <sheet name="Loop" sheetId="15" r:id="rId15"/>
-    <sheet name="Chatham" sheetId="16" r:id="rId16"/>
-    <sheet name="Uptown" sheetId="17" r:id="rId17"/>
+    <sheet name="Rush &amp; Division" sheetId="13" r:id="rId13"/>
+    <sheet name="Loop" sheetId="14" r:id="rId14"/>
+    <sheet name="Chatham" sheetId="15" r:id="rId15"/>
+    <sheet name="Lower West Side" sheetId="16" r:id="rId16"/>
+    <sheet name="Fuller Park" sheetId="17" r:id="rId17"/>
     <sheet name="United Center" sheetId="18" r:id="rId18"/>
     <sheet name="Ashburn" sheetId="19" r:id="rId19"/>
     <sheet name="South Shore" sheetId="20" r:id="rId20"/>
-    <sheet name="River North" sheetId="21" r:id="rId21"/>
-    <sheet name="Austin" sheetId="22" r:id="rId22"/>
-    <sheet name="Wicker Park" sheetId="23" r:id="rId23"/>
-    <sheet name="Lincoln Park" sheetId="24" r:id="rId24"/>
+    <sheet name="Austin" sheetId="21" r:id="rId21"/>
+    <sheet name="Wicker Park" sheetId="22" r:id="rId22"/>
+    <sheet name="Lincoln Park" sheetId="23" r:id="rId23"/>
+    <sheet name="River North" sheetId="24" r:id="rId24"/>
     <sheet name="Printers Row" sheetId="25" r:id="rId25"/>
     <sheet name="Lake View" sheetId="26" r:id="rId26"/>
-    <sheet name="Fuller Park" sheetId="27" r:id="rId27"/>
-    <sheet name="Old Town" sheetId="28" r:id="rId28"/>
-    <sheet name="Logan Square" sheetId="29" r:id="rId29"/>
+    <sheet name="Old Town" sheetId="27" r:id="rId27"/>
+    <sheet name="Logan Square" sheetId="28" r:id="rId28"/>
+    <sheet name="Uptown" sheetId="29" r:id="rId29"/>
     <sheet name="Irving Park" sheetId="30" r:id="rId30"/>
     <sheet name="South Deering" sheetId="31" r:id="rId31"/>
     <sheet name="Chinatown" sheetId="32" r:id="rId32"/>
@@ -53,17 +53,17 @@
     <sheet name="Auburn Gresham" sheetId="44" r:id="rId44"/>
     <sheet name="Douglas" sheetId="45" r:id="rId45"/>
     <sheet name="Chicago Lawn" sheetId="46" r:id="rId46"/>
-    <sheet name="West Loop" sheetId="47" r:id="rId47"/>
-    <sheet name="Lincoln Square" sheetId="48" r:id="rId48"/>
-    <sheet name="Woodlawn" sheetId="49" r:id="rId49"/>
-    <sheet name="Near South Side" sheetId="50" r:id="rId50"/>
-    <sheet name="North Lawndale" sheetId="51" r:id="rId51"/>
-    <sheet name="Bridgeport" sheetId="52" r:id="rId52"/>
-    <sheet name="Hyde Park" sheetId="53" r:id="rId53"/>
-    <sheet name="Calumet Heights" sheetId="54" r:id="rId54"/>
-    <sheet name="Gold Coast" sheetId="55" r:id="rId55"/>
-    <sheet name="Mckinley Park" sheetId="56" r:id="rId56"/>
-    <sheet name="Lower West Side" sheetId="57" r:id="rId57"/>
+    <sheet name="Armour Square" sheetId="47" r:id="rId47"/>
+    <sheet name="West Loop" sheetId="48" r:id="rId48"/>
+    <sheet name="Lincoln Square" sheetId="49" r:id="rId49"/>
+    <sheet name="Woodlawn" sheetId="50" r:id="rId50"/>
+    <sheet name="Near South Side" sheetId="51" r:id="rId51"/>
+    <sheet name="North Lawndale" sheetId="52" r:id="rId52"/>
+    <sheet name="Bridgeport" sheetId="53" r:id="rId53"/>
+    <sheet name="Hyde Park" sheetId="54" r:id="rId54"/>
+    <sheet name="Calumet Heights" sheetId="55" r:id="rId55"/>
+    <sheet name="Gold Coast" sheetId="56" r:id="rId56"/>
+    <sheet name="Mckinley Park" sheetId="57" r:id="rId57"/>
     <sheet name="Washington Heights" sheetId="58" r:id="rId58"/>
     <sheet name="O'Hare" sheetId="59" r:id="rId59"/>
     <sheet name="Jefferson Park" sheetId="60" r:id="rId60"/>
@@ -903,7 +903,7 @@
         <v>202</v>
       </c>
       <c r="J3">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1028,7 +1028,7 @@
         <v>873</v>
       </c>
       <c r="J7">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -1603,184 +1603,6 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1942,6 +1764,231 @@
       </c>
       <c r="J5">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>22</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>44</v>
+      </c>
+      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="E6">
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <v>69</v>
+      </c>
+      <c r="G6">
+        <v>57</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>62</v>
+      </c>
+      <c r="D7">
+        <v>79</v>
+      </c>
+      <c r="E7">
+        <v>92</v>
+      </c>
+      <c r="F7">
+        <v>92</v>
+      </c>
+      <c r="G7">
+        <v>88</v>
+      </c>
+      <c r="H7">
+        <v>118</v>
+      </c>
+      <c r="I7">
+        <v>130</v>
+      </c>
+      <c r="J7">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2005,32 +2052,29 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2038,57 +2082,39 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="H3">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
+      <c r="B4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2101,7 +2127,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
@@ -2110,31 +2136,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="G6">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2142,31 +2168,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E7">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="F7">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="G7">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="H7">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="I7">
-        <v>130</v>
+        <v>24</v>
       </c>
       <c r="J7">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2176,13 +2202,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2234,9 +2260,6 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
@@ -2246,131 +2269,85 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>29</v>
-      </c>
-      <c r="E7">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>26</v>
-      </c>
-      <c r="G7">
-        <v>25</v>
-      </c>
-      <c r="H7">
-        <v>13</v>
-      </c>
-      <c r="I7">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2386,7 +2363,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2434,31 +2411,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -2466,26 +2425,29 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>4</v>
@@ -2493,9 +2455,9 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
@@ -2504,28 +2466,28 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
         <v>9</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -2539,28 +2501,28 @@
         <v>8</v>
       </c>
       <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
         <v>14</v>
       </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="G6">
-        <v>22</v>
-      </c>
       <c r="H6">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J6">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3646,7 +3608,7 @@
         <v>12</v>
       </c>
       <c r="J29">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -4288,7 +4250,7 @@
         <v>130</v>
       </c>
       <c r="J53">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -4466,7 +4428,7 @@
         <v>5</v>
       </c>
       <c r="J61">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -5503,7 +5465,7 @@
         <v>873</v>
       </c>
       <c r="J98">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -5848,63 +5810,81 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>4</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
       <c r="C3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5912,31 +5892,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="G5">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I5">
+        <v>34</v>
+      </c>
+      <c r="J5">
         <v>14</v>
-      </c>
-      <c r="J5">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5944,31 +5924,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="J6">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -5977,6 +5957,148 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6032,64 +6154,34 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
       <c r="F3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6099,46 +6191,37 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6146,173 +6229,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6376,24 +6317,39 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
       <c r="G3">
@@ -6403,14 +6359,20 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -6419,31 +6381,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6451,31 +6413,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>7</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -6830,181 +6792,6 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>13</v>
-      </c>
-      <c r="G5">
-        <v>8</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>9</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>12</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7166,6 +6953,187 @@
       </c>
       <c r="J5">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -7229,20 +7197,29 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -7256,32 +7233,32 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -7290,28 +7267,28 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -7322,31 +7299,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G6">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
         <v>9</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6">
-        <v>7</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -10465,6 +10442,184 @@
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10646,7 +10801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -10785,187 +10940,6 @@
       </c>
       <c r="J5">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -11095,14 +11069,17 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
         <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -11113,32 +11090,38 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
@@ -11147,31 +11130,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11179,31 +11162,31 @@
         <v>6</v>
       </c>
       <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
+      <c r="G6">
         <v>7</v>
       </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
+      <c r="H6">
         <v>8</v>
       </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
       <c r="I6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -11267,32 +11250,17 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11303,32 +11271,29 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -11337,31 +11302,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11369,28 +11334,28 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H6">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -11402,6 +11367,196 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>24</v>
+      </c>
+      <c r="F6">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <v>21</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -11550,7 +11705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -11679,7 +11834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -11815,7 +11970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -11866,149 +12021,6 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -12074,33 +12086,30 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12111,28 +12120,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -12143,28 +12143,28 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-12
</commit_message>
<xml_diff>
--- a/output/cta-violent-crime-full-year.xlsx
+++ b/output/cta-violent-crime-full-year.xlsx
@@ -19,23 +19,23 @@
     <sheet name="Humboldt Park" sheetId="10" r:id="rId10"/>
     <sheet name="South Chicago" sheetId="11" r:id="rId11"/>
     <sheet name="Garfield Park" sheetId="12" r:id="rId12"/>
-    <sheet name="Rush &amp; Division" sheetId="13" r:id="rId13"/>
-    <sheet name="Loop" sheetId="14" r:id="rId14"/>
-    <sheet name="Chatham" sheetId="15" r:id="rId15"/>
-    <sheet name="Lower West Side" sheetId="16" r:id="rId16"/>
-    <sheet name="Fuller Park" sheetId="17" r:id="rId17"/>
+    <sheet name="Armour Square" sheetId="13" r:id="rId13"/>
+    <sheet name="Rush &amp; Division" sheetId="14" r:id="rId14"/>
+    <sheet name="Loop" sheetId="15" r:id="rId15"/>
+    <sheet name="Chatham" sheetId="16" r:id="rId16"/>
+    <sheet name="Uptown" sheetId="17" r:id="rId17"/>
     <sheet name="United Center" sheetId="18" r:id="rId18"/>
     <sheet name="Ashburn" sheetId="19" r:id="rId19"/>
     <sheet name="South Shore" sheetId="20" r:id="rId20"/>
-    <sheet name="Austin" sheetId="21" r:id="rId21"/>
-    <sheet name="Wicker Park" sheetId="22" r:id="rId22"/>
-    <sheet name="Lincoln Park" sheetId="23" r:id="rId23"/>
-    <sheet name="River North" sheetId="24" r:id="rId24"/>
+    <sheet name="River North" sheetId="21" r:id="rId21"/>
+    <sheet name="Austin" sheetId="22" r:id="rId22"/>
+    <sheet name="Wicker Park" sheetId="23" r:id="rId23"/>
+    <sheet name="Lincoln Park" sheetId="24" r:id="rId24"/>
     <sheet name="Printers Row" sheetId="25" r:id="rId25"/>
     <sheet name="Lake View" sheetId="26" r:id="rId26"/>
-    <sheet name="Old Town" sheetId="27" r:id="rId27"/>
-    <sheet name="Logan Square" sheetId="28" r:id="rId28"/>
-    <sheet name="Uptown" sheetId="29" r:id="rId29"/>
+    <sheet name="Fuller Park" sheetId="27" r:id="rId27"/>
+    <sheet name="Old Town" sheetId="28" r:id="rId28"/>
+    <sheet name="Logan Square" sheetId="29" r:id="rId29"/>
     <sheet name="Irving Park" sheetId="30" r:id="rId30"/>
     <sheet name="South Deering" sheetId="31" r:id="rId31"/>
     <sheet name="Chinatown" sheetId="32" r:id="rId32"/>
@@ -53,17 +53,17 @@
     <sheet name="Auburn Gresham" sheetId="44" r:id="rId44"/>
     <sheet name="Douglas" sheetId="45" r:id="rId45"/>
     <sheet name="Chicago Lawn" sheetId="46" r:id="rId46"/>
-    <sheet name="Armour Square" sheetId="47" r:id="rId47"/>
-    <sheet name="West Loop" sheetId="48" r:id="rId48"/>
-    <sheet name="Lincoln Square" sheetId="49" r:id="rId49"/>
-    <sheet name="Woodlawn" sheetId="50" r:id="rId50"/>
-    <sheet name="Near South Side" sheetId="51" r:id="rId51"/>
-    <sheet name="North Lawndale" sheetId="52" r:id="rId52"/>
-    <sheet name="Bridgeport" sheetId="53" r:id="rId53"/>
-    <sheet name="Hyde Park" sheetId="54" r:id="rId54"/>
-    <sheet name="Calumet Heights" sheetId="55" r:id="rId55"/>
-    <sheet name="Gold Coast" sheetId="56" r:id="rId56"/>
-    <sheet name="Mckinley Park" sheetId="57" r:id="rId57"/>
+    <sheet name="West Loop" sheetId="47" r:id="rId47"/>
+    <sheet name="Lincoln Square" sheetId="48" r:id="rId48"/>
+    <sheet name="Woodlawn" sheetId="49" r:id="rId49"/>
+    <sheet name="Near South Side" sheetId="50" r:id="rId50"/>
+    <sheet name="North Lawndale" sheetId="51" r:id="rId51"/>
+    <sheet name="Bridgeport" sheetId="52" r:id="rId52"/>
+    <sheet name="Hyde Park" sheetId="53" r:id="rId53"/>
+    <sheet name="Calumet Heights" sheetId="54" r:id="rId54"/>
+    <sheet name="Gold Coast" sheetId="55" r:id="rId55"/>
+    <sheet name="Mckinley Park" sheetId="56" r:id="rId56"/>
+    <sheet name="Lower West Side" sheetId="57" r:id="rId57"/>
     <sheet name="Washington Heights" sheetId="58" r:id="rId58"/>
     <sheet name="O'Hare" sheetId="59" r:id="rId59"/>
     <sheet name="Jefferson Park" sheetId="60" r:id="rId60"/>
@@ -1603,6 +1603,184 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1764,231 +1942,6 @@
       </c>
       <c r="J5">
         <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>13</v>
-      </c>
-      <c r="I2">
-        <v>14</v>
-      </c>
-      <c r="J2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>17</v>
-      </c>
-      <c r="E3">
-        <v>18</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>26</v>
-      </c>
-      <c r="H3">
-        <v>22</v>
-      </c>
-      <c r="I3">
-        <v>32</v>
-      </c>
-      <c r="J3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>44</v>
-      </c>
-      <c r="D6">
-        <v>49</v>
-      </c>
-      <c r="E6">
-        <v>67</v>
-      </c>
-      <c r="F6">
-        <v>69</v>
-      </c>
-      <c r="G6">
-        <v>57</v>
-      </c>
-      <c r="H6">
-        <v>80</v>
-      </c>
-      <c r="I6">
-        <v>80</v>
-      </c>
-      <c r="J6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>49</v>
-      </c>
-      <c r="C7">
-        <v>62</v>
-      </c>
-      <c r="D7">
-        <v>79</v>
-      </c>
-      <c r="E7">
-        <v>92</v>
-      </c>
-      <c r="F7">
-        <v>92</v>
-      </c>
-      <c r="G7">
-        <v>88</v>
-      </c>
-      <c r="H7">
-        <v>118</v>
-      </c>
-      <c r="I7">
-        <v>130</v>
-      </c>
-      <c r="J7">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2052,29 +2005,32 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2082,39 +2038,57 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2127,7 +2101,7 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -2136,31 +2110,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="F6">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2168,31 +2142,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D7">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="E7">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="F7">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="G7">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="H7">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="I7">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2202,13 +2176,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2260,6 +2234,9 @@
         <v>1</v>
       </c>
       <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
@@ -2269,85 +2246,131 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>26</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>13</v>
+      </c>
+      <c r="I7">
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2363,7 +2386,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -2411,13 +2434,31 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -2425,29 +2466,26 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <v>4</v>
@@ -2455,9 +2493,9 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -2466,28 +2504,28 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -2501,28 +2539,28 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>22</v>
+      </c>
+      <c r="H6">
         <v>14</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>10</v>
       </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>12</v>
-      </c>
       <c r="J6">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -5810,81 +5848,63 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
       <c r="C2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>4</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
+      <c r="G4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5892,31 +5912,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J5">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5924,31 +5944,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="G6">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="J6">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -5957,148 +5977,6 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6154,34 +6032,64 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
       <c r="F3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6191,37 +6099,46 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6229,31 +6146,173 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6317,39 +6376,24 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
@@ -6359,20 +6403,14 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -6381,31 +6419,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6413,31 +6451,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>7</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6792,6 +6830,181 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6953,187 +7166,6 @@
       </c>
       <c r="J5">
         <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6">
-        <v>7</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -7197,29 +7229,20 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
       <c r="C2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -7233,32 +7256,32 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -7267,28 +7290,28 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -7299,31 +7322,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="G6">
-        <v>22</v>
-      </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
       <c r="I6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J6">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -10442,184 +10465,6 @@
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10801,7 +10646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -10940,6 +10785,187 @@
       </c>
       <c r="J5">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -11069,17 +11095,14 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
         <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -11090,38 +11113,32 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -11130,31 +11147,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11162,31 +11179,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -11250,17 +11267,32 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11271,29 +11303,32 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
       <c r="G3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
@@ -11302,31 +11337,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11334,28 +11369,28 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H6">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I6">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -11367,196 +11402,6 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>28</v>
-      </c>
-      <c r="E5">
-        <v>21</v>
-      </c>
-      <c r="F5">
-        <v>35</v>
-      </c>
-      <c r="G5">
-        <v>12</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>29</v>
-      </c>
-      <c r="E6">
-        <v>24</v>
-      </c>
-      <c r="F6">
-        <v>42</v>
-      </c>
-      <c r="G6">
-        <v>18</v>
-      </c>
-      <c r="H6">
-        <v>18</v>
-      </c>
-      <c r="I6">
-        <v>21</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -11705,7 +11550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -11834,7 +11679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -11970,7 +11815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -12021,6 +11866,149 @@
         <v>3</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -12086,30 +12074,33 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -12120,19 +12111,28 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -12143,28 +12143,28 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-29
</commit_message>
<xml_diff>
--- a/output/cta-violent-crime-full-year.xlsx
+++ b/output/cta-violent-crime-full-year.xlsx
@@ -25,27 +25,27 @@
     <sheet name="United Center" sheetId="16" r:id="rId16"/>
     <sheet name="Ashburn" sheetId="17" r:id="rId17"/>
     <sheet name="South Shore" sheetId="18" r:id="rId18"/>
-    <sheet name="Irving Park" sheetId="19" r:id="rId19"/>
-    <sheet name="Lake View" sheetId="20" r:id="rId20"/>
-    <sheet name="Austin" sheetId="21" r:id="rId21"/>
-    <sheet name="River North" sheetId="22" r:id="rId22"/>
-    <sheet name="Fuller Park" sheetId="23" r:id="rId23"/>
-    <sheet name="Old Town" sheetId="24" r:id="rId24"/>
-    <sheet name="Printers Row" sheetId="25" r:id="rId25"/>
-    <sheet name="Lincoln Park" sheetId="26" r:id="rId26"/>
-    <sheet name="Logan Square" sheetId="27" r:id="rId27"/>
-    <sheet name="Belmont Cragin" sheetId="28" r:id="rId28"/>
-    <sheet name="Little Italy, UIC" sheetId="29" r:id="rId29"/>
-    <sheet name="Bucktown" sheetId="30" r:id="rId30"/>
-    <sheet name="Rogers Park" sheetId="31" r:id="rId31"/>
-    <sheet name="Norwood Park" sheetId="32" r:id="rId32"/>
-    <sheet name="South Deering" sheetId="33" r:id="rId33"/>
-    <sheet name="Uptown" sheetId="34" r:id="rId34"/>
-    <sheet name="Chinatown" sheetId="35" r:id="rId35"/>
-    <sheet name="Edgewater" sheetId="36" r:id="rId36"/>
-    <sheet name="Roseland" sheetId="37" r:id="rId37"/>
-    <sheet name="West Pullman" sheetId="38" r:id="rId38"/>
-    <sheet name="Sheffield &amp; DePaul" sheetId="39" r:id="rId39"/>
+    <sheet name="Sheffield &amp; DePaul" sheetId="19" r:id="rId19"/>
+    <sheet name="Edgewater" sheetId="20" r:id="rId20"/>
+    <sheet name="Lake View" sheetId="21" r:id="rId21"/>
+    <sheet name="Austin" sheetId="22" r:id="rId22"/>
+    <sheet name="River North" sheetId="23" r:id="rId23"/>
+    <sheet name="Fuller Park" sheetId="24" r:id="rId24"/>
+    <sheet name="Old Town" sheetId="25" r:id="rId25"/>
+    <sheet name="Printers Row" sheetId="26" r:id="rId26"/>
+    <sheet name="Lincoln Park" sheetId="27" r:id="rId27"/>
+    <sheet name="Logan Square" sheetId="28" r:id="rId28"/>
+    <sheet name="Belmont Cragin" sheetId="29" r:id="rId29"/>
+    <sheet name="Irving Park" sheetId="30" r:id="rId30"/>
+    <sheet name="Little Italy, UIC" sheetId="31" r:id="rId31"/>
+    <sheet name="Bucktown" sheetId="32" r:id="rId32"/>
+    <sheet name="Rogers Park" sheetId="33" r:id="rId33"/>
+    <sheet name="Norwood Park" sheetId="34" r:id="rId34"/>
+    <sheet name="South Deering" sheetId="35" r:id="rId35"/>
+    <sheet name="Uptown" sheetId="36" r:id="rId36"/>
+    <sheet name="Chinatown" sheetId="37" r:id="rId37"/>
+    <sheet name="Roseland" sheetId="38" r:id="rId38"/>
+    <sheet name="West Pullman" sheetId="39" r:id="rId39"/>
     <sheet name="Auburn Gresham" sheetId="40" r:id="rId40"/>
     <sheet name="Albany Park" sheetId="41" r:id="rId41"/>
     <sheet name="Douglas" sheetId="42" r:id="rId42"/>
@@ -54,10 +54,10 @@
     <sheet name="Armour Square" sheetId="45" r:id="rId45"/>
     <sheet name="West Loop" sheetId="46" r:id="rId46"/>
     <sheet name="Lincoln Square" sheetId="47" r:id="rId47"/>
-    <sheet name="Woodlawn" sheetId="48" r:id="rId48"/>
-    <sheet name="Calumet Heights" sheetId="49" r:id="rId49"/>
-    <sheet name="North Lawndale" sheetId="50" r:id="rId50"/>
-    <sheet name="Near South Side" sheetId="51" r:id="rId51"/>
+    <sheet name="Near South Side" sheetId="48" r:id="rId48"/>
+    <sheet name="Woodlawn" sheetId="49" r:id="rId49"/>
+    <sheet name="Calumet Heights" sheetId="50" r:id="rId50"/>
+    <sheet name="North Lawndale" sheetId="51" r:id="rId51"/>
     <sheet name="Bridgeport" sheetId="52" r:id="rId52"/>
     <sheet name="Hyde Park" sheetId="53" r:id="rId53"/>
     <sheet name="Lower West Side" sheetId="54" r:id="rId54"/>
@@ -2760,23 +2760,20 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -2787,33 +2784,33 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+      <c r="F3">
         <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2824,16 +2821,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -2842,7 +2839,7 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -2853,7 +2850,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -2862,22 +2859,22 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5610,13 +5607,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -5665,25 +5662,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -5693,107 +5684,90 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
         <v>10</v>
-      </c>
-      <c r="F5">
-        <v>11</v>
       </c>
       <c r="G5">
         <v>11</v>
       </c>
       <c r="H5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>18</v>
-      </c>
-      <c r="F6">
-        <v>18</v>
-      </c>
-      <c r="G6">
-        <v>19</v>
-      </c>
-      <c r="H6">
-        <v>27</v>
-      </c>
-      <c r="I6">
-        <v>26</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -5857,32 +5831,29 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
       <c r="C2">
         <v>4</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5890,80 +5861,74 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
         <v>7</v>
       </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>7</v>
-      </c>
-      <c r="H3">
-        <v>8</v>
-      </c>
       <c r="I3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>23</v>
-      </c>
       <c r="C5">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G5">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="I5">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J5">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -5971,31 +5936,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E6">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="F6">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H6">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="I6">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J6">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -6059,63 +6024,81 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>4</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
       <c r="C3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6123,31 +6106,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="G5">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I5">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J5">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6155,31 +6138,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="J6">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -6188,6 +6171,190 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>21</v>
+      </c>
+      <c r="J6">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -6355,176 +6522,6 @@
       </c>
       <c r="J6">
         <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>18</v>
-      </c>
-      <c r="G4">
-        <v>12</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <v>17</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>19</v>
-      </c>
-      <c r="F5">
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <v>15</v>
-      </c>
-      <c r="H5">
-        <v>17</v>
-      </c>
-      <c r="I5">
-        <v>19</v>
-      </c>
-      <c r="J5">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -6588,13 +6585,19 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -6605,14 +6608,26 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
       <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6620,28 +6635,28 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -6652,31 +6667,31 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I5">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -6686,13 +6701,13 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -6740,106 +6755,95 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J5">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6903,19 +6907,13 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
@@ -6926,22 +6924,16 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
         <v>1</v>
       </c>
     </row>
@@ -6949,13 +6941,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -6964,31 +6950,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -6999,28 +6985,28 @@
         <v>2</v>
       </c>
       <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
       <c r="F6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -7029,128 +7015,6 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -7207,62 +7071,59 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -7270,28 +7131,28 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J5">
         <v>4</v>
@@ -7302,31 +7163,153 @@
         <v>6</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
         <v>10</v>
       </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
       <c r="C6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>17</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7508,6 +7491,371 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>28</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>17</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7610,7 +7958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -7808,7 +8156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -7936,7 +8284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -8076,7 +8424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -8259,356 +8607,6 @@
       </c>
       <c r="J6">
         <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>12</v>
-      </c>
-      <c r="I7">
-        <v>17</v>
-      </c>
-      <c r="J7">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <v>7</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>11</v>
-      </c>
-      <c r="H5">
-        <v>13</v>
-      </c>
-      <c r="I5">
-        <v>12</v>
-      </c>
-      <c r="J5">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -8672,31 +8670,16 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
       <c r="E2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
         <v>1</v>
       </c>
     </row>
@@ -8705,47 +8688,32 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -8753,7 +8721,7 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>1</v>
       </c>
     </row>
@@ -8762,31 +8730,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H6">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I6">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="J6">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -8794,31 +8762,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="H7">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="I7">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="J7">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -8827,6 +8795,216 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
+      </c>
+      <c r="I6">
+        <v>29</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>31</v>
+      </c>
+      <c r="I7">
+        <v>47</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -8968,184 +9146,6 @@
       </c>
       <c r="J5">
         <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2021</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>9</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -10715,17 +10715,14 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
         <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -10736,38 +10733,35 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
@@ -10776,31 +10770,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -10808,31 +10802,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -10842,13 +10836,13 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -10857,9 +10851,10 @@
     <col min="7" max="7" width="4.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10876,99 +10871,143 @@
         <v>2018</v>
       </c>
       <c r="F1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1">
         <v>2020</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2021</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>2022</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="B2">
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
       <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -11044,13 +11083,13 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
@@ -11059,10 +11098,9 @@
     <col min="7" max="7" width="4.7109375" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11079,152 +11117,99 @@
         <v>2018</v>
       </c>
       <c r="F1" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G1" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H1" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="I1" s="1">
-        <v>2022</v>
-      </c>
-      <c r="J1" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
+      <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>29</v>
-      </c>
-      <c r="E6">
-        <v>24</v>
-      </c>
-      <c r="F6">
-        <v>42</v>
-      </c>
-      <c r="G6">
-        <v>18</v>
-      </c>
-      <c r="H6">
-        <v>18</v>
-      </c>
-      <c r="I6">
-        <v>21</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11288,17 +11273,32 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2">
         <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -11309,22 +11309,22 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
       <c r="G3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -11334,7 +11334,7 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
@@ -11343,31 +11343,31 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -11375,31 +11375,31 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H6">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I6">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>